<commit_message>
Contest 5 GT vs MI
</commit_message>
<xml_diff>
--- a/2024/Next Gen dream 11 2024.xlsx
+++ b/2024/Next Gen dream 11 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EB8AEE-57B2-094B-BC28-C93D2EC9505D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F93F41-E6FD-DC44-B53F-709F0ACAC2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47900" yWindow="4300" windowWidth="32400" windowHeight="18500" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="-50860" yWindow="-820" windowWidth="48760" windowHeight="25040" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="49">
   <si>
     <t>Points</t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>Next Gen DREAM 11</t>
+  </si>
+  <si>
+    <t>PBKS vs DC</t>
+  </si>
+  <si>
+    <t>KKR vs SRH</t>
+  </si>
+  <si>
+    <t>RR vs LSG</t>
+  </si>
+  <si>
+    <t>GT vs MI</t>
+  </si>
+  <si>
+    <t>RCB vs PBKS</t>
   </si>
 </sst>
 </file>
@@ -976,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <pane ySplit="18" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
@@ -1269,13 +1284,13 @@
         <v>0</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="T12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="W12" s="6" t="s">
         <v>0</v>
@@ -1361,47 +1376,63 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3" t="str">
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="G14" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="J14" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H14" s="1">
+        <v>30</v>
+      </c>
+      <c r="J14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="M14" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="P14" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1">
+        <v>70</v>
+      </c>
+      <c r="M14" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="N14" s="1">
+        <v>20</v>
+      </c>
+      <c r="P14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="1"/>
-      <c r="S14" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>40</v>
+      </c>
+      <c r="S14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T14" s="1"/>
-      <c r="V14" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="T14" s="1">
+        <v>50</v>
+      </c>
+      <c r="V14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W14" s="1"/>
-      <c r="Y14" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Z14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z14, ($Z14,$W14,$T14,$Q14,$N14,$K14,$H14,$E14), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z14" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="W14" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1410,47 +1441,63 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="str">
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="G15" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="J15" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>50</v>
+      </c>
+      <c r="J15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="M15" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1">
+        <v>60</v>
+      </c>
+      <c r="M15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="P15" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N15" s="1">
+        <v>100</v>
+      </c>
+      <c r="P15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="S15" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T15" s="1"/>
-      <c r="V15" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>70</v>
+      </c>
+      <c r="S15" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T15" s="1">
+        <v>20</v>
+      </c>
+      <c r="V15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W15" s="1"/>
-      <c r="Y15" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Z15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z15, ($Z15,$W15,$T15,$Q15,$N15,$K15,$H15,$E15), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z15" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="W15" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1459,47 +1506,65 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="str">
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="J16" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>50</v>
+      </c>
+      <c r="J16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="M16" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1">
+        <v>60</v>
+      </c>
+      <c r="M16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="P16" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N16" s="1">
+        <v>30</v>
+      </c>
+      <c r="P16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="S16" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>100</v>
+      </c>
+      <c r="S16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T16" s="1"/>
-      <c r="V16" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T16" s="1">
+        <v>40</v>
+      </c>
+      <c r="V16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W16" s="1"/>
-      <c r="Y16" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="W16" s="1">
+        <v>70</v>
+      </c>
+      <c r="Y16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Z16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z16, ($Z16,$W16,$T16,$Q16,$N16,$K16,$H16,$E16), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z16" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1508,47 +1573,65 @@
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3" t="str">
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>50</v>
+      </c>
+      <c r="G17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="J17" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+      <c r="J17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="M17" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1">
+        <v>70</v>
+      </c>
+      <c r="M17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="P17" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N17" s="1">
+        <v>100</v>
+      </c>
+      <c r="P17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="S17" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>30</v>
+      </c>
+      <c r="S17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T17" s="1"/>
-      <c r="V17" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W17" s="1"/>
-      <c r="Y17" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="W17" s="1">
+        <v>40</v>
+      </c>
+      <c r="Y17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Z17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z17, ($Z17,$W17,$T17,$Q17,$N17,$K17,$H17,$E17), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z17" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1557,7 +1640,9 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D18" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -4311,12 +4396,14 @@
         <v>Sundar</v>
       </c>
       <c r="S74" s="1"/>
-      <c r="T74" s="9" t="s">
-        <v>41</v>
+      <c r="T74" s="9" t="str">
+        <f>S12</f>
+        <v>Sampath</v>
       </c>
       <c r="V74" s="1"/>
-      <c r="W74" s="9" t="s">
-        <v>42</v>
+      <c r="W74" s="9" t="str">
+        <f>V12</f>
+        <v>Jayanth</v>
       </c>
       <c r="Y74" s="1"/>
       <c r="Z74" s="9" t="str">
@@ -4330,56 +4417,56 @@
       </c>
       <c r="E75" s="10">
         <f>SUM(D13:D72)</f>
-        <v>5</v>
+        <v>-30</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="10">
         <f>SUM(G13:G72)</f>
-        <v>-10</v>
+        <v>-55</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="10">
         <f>SUM(J13:J72)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="N75" s="10">
         <f>SUM(M13:M72)</f>
-        <v>-20</v>
+        <v>42.5</v>
       </c>
       <c r="P75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Q75" s="10">
         <f>SUM(P13:P72)</f>
-        <v>-5</v>
+        <v>40</v>
       </c>
       <c r="S75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="10">
         <f>SUM(S13:S72)</f>
-        <v>-25</v>
+        <v>-87.5</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="10">
         <f>SUM(V13:V72)</f>
-        <v>-15</v>
+        <v>30</v>
       </c>
       <c r="Y75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Z75" s="10">
         <f>SUM(Y13:Y72)</f>
-        <v>20</v>
+        <v>-40</v>
       </c>
       <c r="AA75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75,Z75)</f>

</xml_diff>

<commit_message>
Contest 6 RCB vs PBKS
</commit_message>
<xml_diff>
--- a/2024/Next Gen dream 11 2024.xlsx
+++ b/2024/Next Gen dream 11 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CFE25C-A739-5145-851F-DE74265F0461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32DDEF9-EB23-C04C-88A1-242457FEC144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50860" yWindow="-820" windowWidth="48760" windowHeight="25040" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="-48420" yWindow="-2420" windowWidth="48140" windowHeight="26580" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="50">
   <si>
     <t>Points</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>RCB vs PBKS</t>
+  </si>
+  <si>
+    <t>CSK vs GT</t>
   </si>
 </sst>
 </file>
@@ -359,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -386,8 +389,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,10 +398,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -993,7 +995,7 @@
   <dimension ref="A1:AA75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="19" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
@@ -1027,24 +1029,24 @@
       <c r="B2" s="1">
         <v>50</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
     </row>
     <row r="3" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1053,22 +1055,22 @@
       <c r="B3" s="1">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1077,22 +1079,22 @@
       <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1101,22 +1103,22 @@
       <c r="B5" s="1">
         <v>-5</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
     </row>
     <row r="6" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1125,22 +1127,22 @@
       <c r="B6" s="1">
         <v>-10</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1149,22 +1151,22 @@
       <c r="B7" s="1">
         <v>-15</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
     </row>
     <row r="8" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1173,22 +1175,22 @@
       <c r="B8" s="1">
         <v>-20</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1202,15 +1204,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-    </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="18"/>
       <c r="G11" s="19" t="s">
         <v>14</v>
       </c>
@@ -1640,46 +1638,62 @@
       <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="G18" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1">
+        <v>70</v>
+      </c>
+      <c r="G18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="J18" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="H18" s="1">
+        <v>50</v>
+      </c>
+      <c r="J18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="M18" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K18" s="1">
+        <v>20</v>
+      </c>
+      <c r="M18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N18" s="1"/>
-      <c r="P18" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N18" s="1">
+        <v>30</v>
+      </c>
+      <c r="P18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="S18" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T18" s="1"/>
-      <c r="V18" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T18" s="1">
+        <v>40</v>
+      </c>
+      <c r="V18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W18" s="1"/>
-      <c r="Y18" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="W18" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Z18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z18, ($Z18,$W18,$T18,$Q18,$N18,$K18,$H18,$E18), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z18" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1688,7 +1702,9 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="D19" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -4414,56 +4430,56 @@
       </c>
       <c r="E75" s="10">
         <f>SUM(D13:D72)</f>
-        <v>-30</v>
+        <v>-10</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="10">
         <f>SUM(G13:G72)</f>
-        <v>-55</v>
+        <v>-60</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="10">
         <f>SUM(J13:J72)</f>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="M75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="N75" s="10">
         <f>SUM(M13:M72)</f>
-        <v>42.5</v>
+        <v>27.5</v>
       </c>
       <c r="P75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Q75" s="10">
         <f>SUM(P13:P72)</f>
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="S75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="10">
         <f>SUM(S13:S72)</f>
-        <v>-87.5</v>
+        <v>-97.5</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="10">
         <f>SUM(V13:V72)</f>
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="Y75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Z75" s="10">
         <f>SUM(Y13:Y72)</f>
-        <v>-40</v>
+        <v>-35</v>
       </c>
       <c r="AA75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75,Z75)</f>
@@ -4473,6 +4489,7 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="9">
+    <mergeCell ref="Y11:Z11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="J11:K11"/>
@@ -4481,7 +4498,6 @@
     <mergeCell ref="S11:T11"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="V11:W11"/>
-    <mergeCell ref="Y11:Z11"/>
   </mergeCells>
   <conditionalFormatting sqref="E75">
     <cfRule type="cellIs" dxfId="26" priority="141" operator="greaterThan">

</xml_diff>

<commit_message>
Contest 7 CSK vs GT
</commit_message>
<xml_diff>
--- a/2024/Next Gen dream 11 2024.xlsx
+++ b/2024/Next Gen dream 11 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32DDEF9-EB23-C04C-88A1-242457FEC144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2538F775-434E-9846-ACA7-3684BE6E7301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48420" yWindow="-2420" windowWidth="48140" windowHeight="26580" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="-49020" yWindow="-2500" windowWidth="46120" windowHeight="26560" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="51">
   <si>
     <t>Points</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>CSK vs GT</t>
+  </si>
+  <si>
+    <t>SRH vs MI</t>
   </si>
 </sst>
 </file>
@@ -994,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <pane ySplit="19" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="20" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
@@ -1705,46 +1708,62 @@
       <c r="C19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="G19" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>50</v>
+      </c>
+      <c r="G19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="J19" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
+        <v>70</v>
+      </c>
+      <c r="J19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="M19" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="P19" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N19" s="1">
+        <v>30</v>
+      </c>
+      <c r="P19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="S19" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>60</v>
+      </c>
+      <c r="S19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T19" s="1"/>
-      <c r="V19" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="T19" s="1">
+        <v>40</v>
+      </c>
+      <c r="V19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W19" s="1"/>
-      <c r="Y19" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="W19" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Z19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z19, ($Z19,$W19,$T19,$Q19,$N19,$K19,$H19,$E19), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z19" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1753,7 +1772,9 @@
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D20" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -4430,56 +4451,56 @@
       </c>
       <c r="E75" s="10">
         <f>SUM(D13:D72)</f>
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="10">
         <f>SUM(G13:G72)</f>
-        <v>-60</v>
+        <v>-40</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="10">
         <f>SUM(J13:J72)</f>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="M75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="N75" s="10">
         <f>SUM(M13:M72)</f>
-        <v>27.5</v>
+        <v>12.5</v>
       </c>
       <c r="P75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Q75" s="10">
         <f>SUM(P13:P72)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="10">
         <f>SUM(S13:S72)</f>
-        <v>-97.5</v>
+        <v>-107.5</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="10">
         <f>SUM(V13:V72)</f>
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="Y75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Z75" s="10">
         <f>SUM(Y13:Y72)</f>
-        <v>-35</v>
+        <v>-55</v>
       </c>
       <c r="AA75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75,Z75)</f>

</xml_diff>

<commit_message>
Contest 8 SRH vs MI
</commit_message>
<xml_diff>
--- a/2024/Next Gen dream 11 2024.xlsx
+++ b/2024/Next Gen dream 11 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2538F775-434E-9846-ACA7-3684BE6E7301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CD08DB-FE80-A740-B590-724B9B298658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49020" yWindow="-2500" windowWidth="46120" windowHeight="26560" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="-49020" yWindow="-2500" windowWidth="47880" windowHeight="26560" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="69">
   <si>
     <t>Points</t>
   </si>
@@ -195,6 +195,60 @@
   </si>
   <si>
     <t>SRH vs MI</t>
+  </si>
+  <si>
+    <t>RR vs DC</t>
+  </si>
+  <si>
+    <t>RCB vs KKR</t>
+  </si>
+  <si>
+    <t>LSG vs PBKS</t>
+  </si>
+  <si>
+    <t>GT vs SRH</t>
+  </si>
+  <si>
+    <t>DC vs CSK</t>
+  </si>
+  <si>
+    <t>MI vs RR</t>
+  </si>
+  <si>
+    <t>RCB vs LSG</t>
+  </si>
+  <si>
+    <t>DC vs KKR</t>
+  </si>
+  <si>
+    <t>GT vs PBKS</t>
+  </si>
+  <si>
+    <t>SRH vs CSK</t>
+  </si>
+  <si>
+    <t>RR vs RCB</t>
+  </si>
+  <si>
+    <t>MI vs DC</t>
+  </si>
+  <si>
+    <t>LSG vs GT</t>
+  </si>
+  <si>
+    <t>CSK vs KKR</t>
+  </si>
+  <si>
+    <t>PBKS vs SRH</t>
+  </si>
+  <si>
+    <t>RR vs GT</t>
+  </si>
+  <si>
+    <t>MI vs RCB</t>
+  </si>
+  <si>
+    <t>LSG vs DC</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1052,7 @@
   <dimension ref="A1:AA75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="20" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="20" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
@@ -1775,46 +1829,62 @@
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="3" t="str">
+        <v>-5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="G20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(H20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="J20" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H20" s="1">
+        <v>30</v>
+      </c>
+      <c r="J20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(K20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="M20" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>40</v>
+      </c>
+      <c r="M20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(N20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="P20" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="N20" s="1">
+        <v>60</v>
+      </c>
+      <c r="P20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Q20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="1"/>
-      <c r="S20" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>70</v>
+      </c>
+      <c r="S20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(T20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T20" s="1"/>
-      <c r="V20" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(W20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(W20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="W20" s="1"/>
-      <c r="Y20" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="W20" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Z20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(Z20, ($Z20,$W20,$T20,$Q20,$N20,$K20,$H20,$E20), 0),  $A$2:$B$10, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Z20" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1823,7 +1893,9 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="D21" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($Z21,$W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E21, ($Z21,$W21,$T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -1872,7 +1944,9 @@
       <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="D22" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E22, ($Z22,$W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E22, ($Z22,$W22,$T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -1921,7 +1995,9 @@
       <c r="B23" s="4">
         <v>1</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="D23" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($Z23,$W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E23, ($Z23,$W23,$T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -1970,7 +2046,9 @@
       <c r="B24" s="4">
         <v>1</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="D24" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E24, ($Z24,$W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E24, ($Z24,$W24,$T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2019,7 +2097,9 @@
       <c r="B25" s="4">
         <v>1</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="D25" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E25, ($Z25,$W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E25, ($Z25,$W25,$T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2068,7 +2148,9 @@
       <c r="B26" s="4">
         <v>1</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D26" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E26, ($Z26,$W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E26, ($Z26,$W26,$T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2117,7 +2199,9 @@
       <c r="B27" s="4">
         <v>1</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="D27" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E27, ($Z27,$W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E27, ($Z27,$W27,$T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2166,7 +2250,9 @@
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="14"/>
+      <c r="C28" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="D28" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E28, ($Z28,$W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E28, ($Z28,$W28,$T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2215,7 +2301,9 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="D29" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($Z29,$W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E29, ($Z29,$W29,$T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2264,7 +2352,9 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="14" t="s">
+        <v>60</v>
+      </c>
       <c r="D30" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E30, ($Z30,$W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E30, ($Z30,$W30,$T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2313,7 +2403,9 @@
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="D31" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($Z31,$W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E31, ($Z31,$W31,$T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2362,7 +2454,9 @@
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="14"/>
+      <c r="C32" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="D32" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($Z32,$W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E32, ($Z32,$W32,$T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2411,7 +2505,9 @@
       <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="14"/>
+      <c r="C33" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D33" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E33, ($Z33,$W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E33, ($Z33,$W33,$T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2460,7 +2556,9 @@
       <c r="B34" s="1">
         <v>1</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="D34" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E34, ($Z34,$W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E34, ($Z34,$W34,$T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2509,7 +2607,9 @@
       <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="14"/>
+      <c r="C35" s="14" t="s">
+        <v>65</v>
+      </c>
       <c r="D35" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E35, ($Z35,$W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E35, ($Z35,$W35,$T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2558,7 +2658,9 @@
       <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="14"/>
+      <c r="C36" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="D36" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E36, ($Z36,$W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E36, ($Z36,$W36,$T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2607,7 +2709,9 @@
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="D37" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E37, ($Z37,$W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E37, ($Z37,$W37,$T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -2656,7 +2760,9 @@
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="D38" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E38, ($Z38,$W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE)),"",VLOOKUP(RANK(E38, ($Z38,$W38,$T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$B$10, 2, FALSE))</f>
         <v/>
@@ -4451,56 +4557,56 @@
       </c>
       <c r="E75" s="10">
         <f>SUM(D13:D72)</f>
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H75" s="10">
         <f>SUM(G13:G72)</f>
-        <v>-40</v>
+        <v>-55</v>
       </c>
       <c r="J75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="K75" s="10">
         <f>SUM(J13:J72)</f>
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="M75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="N75" s="10">
         <f>SUM(M13:M72)</f>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
       <c r="P75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Q75" s="10">
         <f>SUM(P13:P72)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="S75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T75" s="10">
         <f>SUM(S13:S72)</f>
-        <v>-107.5</v>
+        <v>-132.5</v>
       </c>
       <c r="V75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="W75" s="10">
         <f>SUM(V13:V72)</f>
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="Y75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Z75" s="10">
         <f>SUM(Y13:Y72)</f>
-        <v>-55</v>
+        <v>-75</v>
       </c>
       <c r="AA75" s="1">
         <f>SUM(E75,H75,K75,N75,Q75,T75,W75,Z75)</f>

</xml_diff>